<commit_message>
Baase of backend 0.0
</commit_message>
<xml_diff>
--- a/APP_PLAN.xlsx
+++ b/APP_PLAN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ax07057\PROGRAMOK\XAMPP\xampp\htdocs\DNTST_REG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B51185E-B5A5-418A-A586-FD6691AD6B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D0304D-5361-4E40-85B7-6CC0F67B632C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{97BD8106-7FB7-4877-91D7-B534E09B47E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{97BD8106-7FB7-4877-91D7-B534E09B47E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -1372,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC197D14-36A5-4124-82BD-244C6A01C3FB}">
   <dimension ref="B3:P122"/>
   <sheetViews>
-    <sheetView topLeftCell="B25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AK53" sqref="AK53"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3200,8 +3200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9462A544-5864-433A-9BAF-B073476BD8D0}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I53" sqref="I3:I53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Excel temp file cleared
</commit_message>
<xml_diff>
--- a/APP_PLAN.xlsx
+++ b/APP_PLAN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ax07057\PROGRAMOK\XAMPP\xampp\htdocs\DNTST_REG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D0304D-5361-4E40-85B7-6CC0F67B632C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB39AED-32DB-4234-A74B-7C11871A1889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{97BD8106-7FB7-4877-91D7-B534E09B47E7}"/>
   </bookViews>
@@ -1372,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC197D14-36A5-4124-82BD-244C6A01C3FB}">
   <dimension ref="B3:P122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>